<commit_message>
update of some data extraction files in relation to Task 4.4 analysis
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Festjens.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Festjens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1B3740-771B-4766-B640-7B53B20EE1BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4615361-F962-4652-9EF4-D443B09D118D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4918,10 +4918,10 @@
   <dimension ref="A1:AY81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AY64" sqref="AY64"/>
+      <selection pane="bottomRight" activeCell="AK48" sqref="AK48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10574,7 +10574,7 @@
         <v>120</v>
       </c>
       <c r="AJ45" s="12" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="AK45" s="12" t="s">
         <v>156</v>
@@ -11131,7 +11131,7 @@
         <v>120</v>
       </c>
       <c r="AJ49" s="12" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="AK49" s="12" t="s">
         <v>156</v>
@@ -11688,7 +11688,7 @@
         <v>120</v>
       </c>
       <c r="AJ53" s="12" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="AK53" s="12" t="s">
         <v>156</v>
@@ -15211,7 +15211,7 @@
       <formula1>Fishery_type</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="Q3:Q1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ3:AK1048576 AO3:AO1048576 AS3:AT1048576" xr:uid="{E3465DE4-B915-4C62-9316-EABEC40DC1E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS3:AT1048576 AO3:AO1048576 AJ3:AK1048576" xr:uid="{E3465DE4-B915-4C62-9316-EABEC40DC1E6}">
       <formula1>INDIRECT(AI3)</formula1>
     </dataValidation>
   </dataValidations>
@@ -17308,9 +17308,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17428,25 +17431,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17468,9 +17461,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update data extraction files and cleaned dataset
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Festjens.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Festjens.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585B0784-F37C-454B-882C-106DF2642AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB8CDF6-529F-4184-8880-3EC90196F132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -4927,7 +4927,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AQ77" sqref="AQ77"/>
+      <selection pane="bottomRight" activeCell="AX86" sqref="AX86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12861,7 +12861,7 @@
         <v>213</v>
       </c>
       <c r="AX62" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AY62" s="12" t="s">
         <v>515</v>
@@ -12986,7 +12986,7 @@
         <v>213</v>
       </c>
       <c r="AX63" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AY63" s="12" t="s">
         <v>515</v>
@@ -14242,7 +14242,7 @@
         <v>113</v>
       </c>
       <c r="AX73" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AY73" s="12" t="s">
         <v>513</v>
@@ -17445,21 +17445,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abe771af6212f3f785694fa6f4ad1686">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -17573,30 +17558,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17610,4 +17587,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update data extraction files and process methods columns
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Festjens.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Festjens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D1D2E4-42F0-46FE-B82A-2EF4B5B4609F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF963576-E6F1-4BBF-B543-7F6DBB61D4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4650" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3651" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3651" uniqueCount="629">
   <si>
     <t>SearchID</t>
   </si>
@@ -4367,9 +4367,6 @@
     </r>
   </si>
   <si>
-    <t>SST data _ plankton data _ cod data</t>
-  </si>
-  <si>
     <t>For production, both sand and gravel habitats showed fast recovery (less than 2 years) throughout most of the area, whereas a small fraction of the area recovered after about 7 years. Mud habitat recovered within 4 years. A large fraction of the muddy sand habitat recovered in about 2 years, whereas the majority of this habitat had recovered after 5 years. The areas that recovered most slowly were sand and gravel areas in the northwestern North Sea. Recovery trajectories
 for the biomass state indicator were similar to those for the production indicator, but recovery generally took twice as long.</t>
   </si>
@@ -4423,6 +4420,15 @@
   </si>
   <si>
     <t>litter ingestion</t>
+  </si>
+  <si>
+    <t>Continuous Plankton Recorder</t>
+  </si>
+  <si>
+    <t>ICES stock assessment database</t>
+  </si>
+  <si>
+    <t>Continuous Plankton Recorder _ ICES stock assessment database</t>
   </si>
 </sst>
 </file>
@@ -4928,31 +4934,31 @@
   <dimension ref="A1:AY83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AP84" sqref="AP84"/>
+      <selection pane="bottomRight" activeCell="AB87" sqref="AB87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.453125" customWidth="1"/>
-    <col min="20" max="20" width="18.1796875" customWidth="1"/>
-    <col min="25" max="26" width="32.81640625" customWidth="1"/>
-    <col min="35" max="36" width="17.81640625" customWidth="1"/>
-    <col min="37" max="37" width="18.81640625" customWidth="1"/>
-    <col min="38" max="38" width="19.1796875" customWidth="1"/>
-    <col min="39" max="39" width="17.81640625" customWidth="1"/>
-    <col min="40" max="40" width="14.1796875" customWidth="1"/>
-    <col min="41" max="42" width="15.81640625" customWidth="1"/>
-    <col min="43" max="43" width="15.453125" customWidth="1"/>
-    <col min="47" max="47" width="15.1796875" customWidth="1"/>
-    <col min="48" max="48" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1"/>
+    <col min="25" max="26" width="32.85546875" customWidth="1"/>
+    <col min="35" max="36" width="17.85546875" customWidth="1"/>
+    <col min="37" max="37" width="18.85546875" customWidth="1"/>
+    <col min="38" max="38" width="19.140625" customWidth="1"/>
+    <col min="39" max="39" width="17.85546875" customWidth="1"/>
+    <col min="40" max="40" width="14.140625" customWidth="1"/>
+    <col min="41" max="42" width="15.85546875" customWidth="1"/>
+    <col min="43" max="43" width="15.42578125" customWidth="1"/>
+    <col min="47" max="47" width="15.140625" customWidth="1"/>
+    <col min="48" max="48" width="18.85546875" customWidth="1"/>
     <col min="49" max="49" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>476</v>
       </c>
@@ -5021,7 +5027,7 @@
       <c r="AX1" s="15"/>
       <c r="AY1" s="15"/>
     </row>
-    <row r="2" spans="1:51" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
@@ -5173,7 +5179,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>477</v>
       </c>
@@ -5304,7 +5310,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>477</v>
       </c>
@@ -5435,7 +5441,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>477</v>
       </c>
@@ -5503,7 +5509,7 @@
         <v>113</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>608</v>
+        <v>626</v>
       </c>
       <c r="AA5" s="11" t="s">
         <v>517</v>
@@ -5557,7 +5563,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="6" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>477</v>
       </c>
@@ -5625,7 +5631,7 @@
         <v>113</v>
       </c>
       <c r="Z6" s="11" t="s">
-        <v>608</v>
+        <v>627</v>
       </c>
       <c r="AA6" s="11" t="s">
         <v>517</v>
@@ -5676,7 +5682,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="7" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>477</v>
       </c>
@@ -5744,7 +5750,7 @@
         <v>113</v>
       </c>
       <c r="Z7" s="11" t="s">
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="AA7" s="11" t="s">
         <v>517</v>
@@ -5789,7 +5795,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="8" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>477</v>
       </c>
@@ -5857,7 +5863,7 @@
         <v>113</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>608</v>
+        <v>626</v>
       </c>
       <c r="AA8" s="11" t="s">
         <v>517</v>
@@ -5902,7 +5908,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="9" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>477</v>
       </c>
@@ -6033,7 +6039,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="10" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>477</v>
       </c>
@@ -6164,7 +6170,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="11" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>477</v>
       </c>
@@ -6295,7 +6301,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="12" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>477</v>
       </c>
@@ -6417,7 +6423,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="13" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>477</v>
       </c>
@@ -6539,7 +6545,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="14" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>477</v>
       </c>
@@ -6661,7 +6667,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="15" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>477</v>
       </c>
@@ -6780,7 +6786,7 @@
         <v>527</v>
       </c>
       <c r="AV15" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AW15" s="11" t="s">
         <v>199</v>
@@ -6792,7 +6798,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="16" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>477</v>
       </c>
@@ -6905,7 +6911,7 @@
         <v>480</v>
       </c>
       <c r="AQ16" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AR16" s="11" t="s">
         <v>164</v>
@@ -6930,7 +6936,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="17" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>477</v>
       </c>
@@ -7070,7 +7076,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="18" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>477</v>
       </c>
@@ -7204,7 +7210,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="19" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>477</v>
       </c>
@@ -7338,7 +7344,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="20" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>477</v>
       </c>
@@ -7460,10 +7466,10 @@
         <v>208</v>
       </c>
       <c r="AY20" s="11" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
-    <row r="21" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>477</v>
       </c>
@@ -7585,10 +7591,10 @@
         <v>207</v>
       </c>
       <c r="AY21" s="11" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
-    <row r="22" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>477</v>
       </c>
@@ -7683,7 +7689,7 @@
         <v>232</v>
       </c>
       <c r="AP22" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AR22" s="11" t="s">
         <v>164</v>
@@ -7692,7 +7698,7 @@
         <v>239</v>
       </c>
       <c r="AV22" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AW22" s="11" t="s">
         <v>199</v>
@@ -7704,7 +7710,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="23" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>477</v>
       </c>
@@ -7799,7 +7805,7 @@
         <v>232</v>
       </c>
       <c r="AP23" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AR23" s="11" t="s">
         <v>164</v>
@@ -7808,7 +7814,7 @@
         <v>240</v>
       </c>
       <c r="AV23" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AW23" s="11" t="s">
         <v>199</v>
@@ -7820,7 +7826,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="24" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>477</v>
       </c>
@@ -7915,7 +7921,7 @@
         <v>232</v>
       </c>
       <c r="AP24" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AR24" s="11" t="s">
         <v>164</v>
@@ -7927,7 +7933,7 @@
         <v>181</v>
       </c>
       <c r="AV24" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AW24" s="11" t="s">
         <v>199</v>
@@ -7939,7 +7945,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="25" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>477</v>
       </c>
@@ -8052,7 +8058,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="26" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>477</v>
       </c>
@@ -8180,7 +8186,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="27" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>477</v>
       </c>
@@ -8308,7 +8314,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="28" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>477</v>
       </c>
@@ -8436,7 +8442,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="29" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>477</v>
       </c>
@@ -8564,7 +8570,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="30" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>477</v>
       </c>
@@ -8692,7 +8698,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="31" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>477</v>
       </c>
@@ -8820,7 +8826,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="32" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>477</v>
       </c>
@@ -8948,7 +8954,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="33" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>477</v>
       </c>
@@ -9076,7 +9082,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="34" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>477</v>
       </c>
@@ -9190,7 +9196,7 @@
       </c>
       <c r="AU34" s="13"/>
       <c r="AV34" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AW34" s="11" t="s">
         <v>204</v>
@@ -9199,10 +9205,10 @@
         <v>209</v>
       </c>
       <c r="AY34" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="35" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>477</v>
       </c>
@@ -9315,7 +9321,7 @@
         <v>176</v>
       </c>
       <c r="AV35" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AW35" s="11" t="s">
         <v>204</v>
@@ -9324,10 +9330,10 @@
         <v>209</v>
       </c>
       <c r="AY35" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="36" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>477</v>
       </c>
@@ -9440,7 +9446,7 @@
         <v>176</v>
       </c>
       <c r="AV36" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AW36" s="11" t="s">
         <v>204</v>
@@ -9449,10 +9455,10 @@
         <v>209</v>
       </c>
       <c r="AY36" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="37" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>477</v>
       </c>
@@ -9565,7 +9571,7 @@
         <v>176</v>
       </c>
       <c r="AV37" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AW37" s="11" t="s">
         <v>204</v>
@@ -9574,10 +9580,10 @@
         <v>209</v>
       </c>
       <c r="AY37" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="38" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>477</v>
       </c>
@@ -9691,7 +9697,7 @@
       </c>
       <c r="AU38" s="13"/>
       <c r="AV38" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AW38" s="11" t="s">
         <v>199</v>
@@ -9700,10 +9706,10 @@
         <v>209</v>
       </c>
       <c r="AY38" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="39" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>477</v>
       </c>
@@ -9816,7 +9822,7 @@
         <v>176</v>
       </c>
       <c r="AV39" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AW39" s="11" t="s">
         <v>199</v>
@@ -9825,10 +9831,10 @@
         <v>209</v>
       </c>
       <c r="AY39" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="40" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>477</v>
       </c>
@@ -9941,7 +9947,7 @@
         <v>176</v>
       </c>
       <c r="AV40" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AW40" s="11" t="s">
         <v>199</v>
@@ -9950,10 +9956,10 @@
         <v>209</v>
       </c>
       <c r="AY40" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="41" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>477</v>
       </c>
@@ -10066,7 +10072,7 @@
         <v>176</v>
       </c>
       <c r="AV41" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AW41" s="11" t="s">
         <v>199</v>
@@ -10075,10 +10081,10 @@
         <v>209</v>
       </c>
       <c r="AY41" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="42" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>477</v>
       </c>
@@ -10218,7 +10224,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="43" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>477</v>
       </c>
@@ -10358,7 +10364,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="44" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>477</v>
       </c>
@@ -10495,7 +10501,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="45" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>477</v>
       </c>
@@ -10635,7 +10641,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="46" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>477</v>
       </c>
@@ -10775,7 +10781,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="47" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>477</v>
       </c>
@@ -10915,7 +10921,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="48" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>477</v>
       </c>
@@ -11052,7 +11058,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="49" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>477</v>
       </c>
@@ -11192,7 +11198,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="50" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>477</v>
       </c>
@@ -11332,7 +11338,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="51" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>477</v>
       </c>
@@ -11472,7 +11478,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="52" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>477</v>
       </c>
@@ -11609,7 +11615,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="53" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>477</v>
       </c>
@@ -11749,7 +11755,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="54" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>477</v>
       </c>
@@ -11874,7 +11880,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="55" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>477</v>
       </c>
@@ -11999,7 +12005,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="56" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>477</v>
       </c>
@@ -12121,7 +12127,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="57" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>477</v>
       </c>
@@ -12246,7 +12252,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="58" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>477</v>
       </c>
@@ -12380,7 +12386,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="59" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>477</v>
       </c>
@@ -12487,7 +12493,7 @@
         <v>233</v>
       </c>
       <c r="AP59" s="11" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AR59" s="11" t="s">
         <v>164</v>
@@ -12508,7 +12514,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="60" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>477</v>
       </c>
@@ -12612,7 +12618,7 @@
         <v>231</v>
       </c>
       <c r="AP60" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="AR60" s="11" t="s">
         <v>150</v>
@@ -12621,7 +12627,7 @@
         <v>197</v>
       </c>
       <c r="AV60" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AW60" s="11" t="s">
         <v>238</v>
@@ -12630,10 +12636,10 @@
         <v>210</v>
       </c>
       <c r="AY60" s="11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
-    <row r="61" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>477</v>
       </c>
@@ -12737,7 +12743,7 @@
         <v>231</v>
       </c>
       <c r="AP61" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="AR61" s="11" t="s">
         <v>150</v>
@@ -12746,7 +12752,7 @@
         <v>170</v>
       </c>
       <c r="AV61" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AW61" s="11" t="s">
         <v>238</v>
@@ -12755,10 +12761,10 @@
         <v>210</v>
       </c>
       <c r="AY61" s="11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
-    <row r="62" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>477</v>
       </c>
@@ -12886,7 +12892,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="63" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>477</v>
       </c>
@@ -13011,7 +13017,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="64" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>477</v>
       </c>
@@ -13133,7 +13139,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="65" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>477</v>
       </c>
@@ -13255,7 +13261,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="66" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>477</v>
       </c>
@@ -13356,7 +13362,7 @@
         <v>233</v>
       </c>
       <c r="AP66" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AR66" s="11" t="s">
         <v>164</v>
@@ -13380,7 +13386,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="67" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>477</v>
       </c>
@@ -13481,7 +13487,7 @@
         <v>233</v>
       </c>
       <c r="AP67" s="11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AR67" s="11" t="s">
         <v>164</v>
@@ -13502,10 +13508,10 @@
         <v>209</v>
       </c>
       <c r="AY67" s="11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
-    <row r="68" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>477</v>
       </c>
@@ -13633,7 +13639,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="69" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>477</v>
       </c>
@@ -13749,7 +13755,7 @@
         <v>515</v>
       </c>
       <c r="AV69" s="11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AW69" s="11" t="s">
         <v>199</v>
@@ -13761,7 +13767,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="70" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>477</v>
       </c>
@@ -13877,7 +13883,7 @@
         <v>515</v>
       </c>
       <c r="AV70" s="11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AW70" s="11" t="s">
         <v>205</v>
@@ -13889,7 +13895,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="71" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>477</v>
       </c>
@@ -14014,7 +14020,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="72" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>477</v>
       </c>
@@ -14139,7 +14145,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="73" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>477</v>
       </c>
@@ -14264,7 +14270,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="74" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>477</v>
       </c>
@@ -14392,7 +14398,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="75" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>477</v>
       </c>
@@ -14517,7 +14523,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="76" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>477</v>
       </c>
@@ -14633,7 +14639,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="77" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>477</v>
       </c>
@@ -14749,7 +14755,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="78" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>477</v>
       </c>
@@ -14853,7 +14859,7 @@
         <v>239</v>
       </c>
       <c r="AV78" s="11" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AW78" s="11" t="s">
         <v>206</v>
@@ -14862,10 +14868,10 @@
         <v>209</v>
       </c>
       <c r="AY78" s="11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="79" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>477</v>
       </c>
@@ -14984,7 +14990,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="80" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>477</v>
       </c>
@@ -15103,7 +15109,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="81" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>477</v>
       </c>
@@ -15210,7 +15216,7 @@
         <v>239</v>
       </c>
       <c r="AV81" s="11" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AW81" s="11" t="s">
         <v>206</v>
@@ -15219,10 +15225,10 @@
         <v>209</v>
       </c>
       <c r="AY81" s="11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="82" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>477</v>
       </c>
@@ -15349,7 +15355,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="83" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>477</v>
       </c>
@@ -15606,17 +15612,17 @@
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="32.1796875" customWidth="1"/>
-    <col min="23" max="23" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.140625" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="32" max="32" width="14.81640625" customWidth="1"/>
-    <col min="33" max="33" width="26.1796875" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="33" max="33" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
@@ -15682,7 +15688,7 @@
       <c r="AW1" s="8"/>
       <c r="AX1" s="8"/>
     </row>
-    <row r="2" spans="1:50" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -15834,7 +15840,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="Q3" t="s">
         <v>21</v>
       </c>
@@ -15891,7 +15897,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="Q4" t="s">
         <v>22</v>
       </c>
@@ -15948,7 +15954,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R5" t="s">
         <v>83</v>
       </c>
@@ -16004,7 +16010,7 @@
       </c>
       <c r="AX5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="R6" t="s">
         <v>84</v>
       </c>
@@ -16049,7 +16055,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R7" t="s">
         <v>85</v>
       </c>
@@ -16091,7 +16097,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R8" t="s">
         <v>86</v>
       </c>
@@ -16129,7 +16135,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R9" t="s">
         <v>87</v>
       </c>
@@ -16164,7 +16170,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
         <v>33</v>
       </c>
@@ -16196,7 +16202,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S11" t="s">
         <v>32</v>
       </c>
@@ -16231,7 +16237,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S12" t="s">
         <v>30</v>
       </c>
@@ -16263,7 +16269,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S13" t="s">
         <v>79</v>
       </c>
@@ -16298,7 +16304,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S14" t="s">
         <v>31</v>
       </c>
@@ -16327,7 +16333,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S15" t="s">
         <v>35</v>
       </c>
@@ -16356,7 +16362,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S16" t="s">
         <v>34</v>
       </c>
@@ -16376,7 +16382,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="17" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AM17" t="s">
         <v>162</v>
       </c>
@@ -16384,22 +16390,22 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="18" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AQ18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="19" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AQ19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="22" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH22" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="23" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH23" s="6" t="s">
         <v>115</v>
       </c>
@@ -16434,7 +16440,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="24" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH24" t="s">
         <v>129</v>
       </c>
@@ -16460,7 +16466,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="25" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH25" t="s">
         <v>137</v>
       </c>
@@ -16483,7 +16489,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="26" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AJ26" t="s">
         <v>144</v>
       </c>
@@ -16494,7 +16500,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="27" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AJ27" t="s">
         <v>147</v>
       </c>
@@ -16505,7 +16511,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="28" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AJ28" t="s">
         <v>149</v>
       </c>
@@ -16513,12 +16519,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="29" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AQ29" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="30" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH30" s="5" t="s">
         <v>151</v>
       </c>
@@ -16541,7 +16547,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="31" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH31" s="6" t="s">
         <v>129</v>
       </c>
@@ -16567,7 +16573,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="32" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH32" t="s">
         <v>153</v>
       </c>
@@ -16593,7 +16599,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="33" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH33" t="s">
         <v>155</v>
       </c>
@@ -16613,7 +16619,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="34" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AI34" t="s">
         <v>157</v>
       </c>
@@ -16627,7 +16633,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="35" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AI35" t="s">
         <v>113</v>
       </c>
@@ -16641,7 +16647,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="36" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AU36" t="s">
         <v>211</v>
       </c>
@@ -16649,10 +16655,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="37" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AL37" s="5"/>
     </row>
-    <row r="38" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="38" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -16680,38 +16686,38 @@
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
     <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.54296875" customWidth="1"/>
-    <col min="17" max="17" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.81640625" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" customWidth="1"/>
-    <col min="20" max="20" width="19.1796875" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" customWidth="1"/>
-    <col min="22" max="22" width="18.81640625" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.453125" customWidth="1"/>
-    <col min="30" max="30" width="15.1796875" customWidth="1"/>
-    <col min="31" max="31" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.81640625" customWidth="1"/>
-    <col min="33" max="33" width="12.54296875" customWidth="1"/>
+    <col min="28" max="28" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" customWidth="1"/>
+    <col min="31" max="31" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -16758,7 +16764,7 @@
       <c r="AF1" s="15"/>
       <c r="AG1" s="15"/>
     </row>
-    <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -16859,7 +16865,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -16925,7 +16931,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -16976,7 +16982,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -17030,7 +17036,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -17072,7 +17078,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -17117,7 +17123,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -17155,7 +17161,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -17193,7 +17199,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -17228,7 +17234,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -17260,7 +17266,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -17292,7 +17298,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -17321,7 +17327,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -17344,7 +17350,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>35</v>
       </c>
@@ -17370,7 +17376,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -17387,7 +17393,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
         <v>119</v>
       </c>
@@ -17398,7 +17404,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q18" t="s">
         <v>120</v>
       </c>
@@ -17412,7 +17418,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R19" t="s">
         <v>152</v>
       </c>
@@ -17426,7 +17432,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S20" t="s">
         <v>156</v>
       </c>
@@ -17437,7 +17443,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S21" t="s">
         <v>228</v>
       </c>
@@ -17451,7 +17457,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S22" t="s">
         <v>113</v>
       </c>
@@ -17462,7 +17468,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q23" t="s">
         <v>127</v>
       </c>
@@ -17476,7 +17482,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R24" t="s">
         <v>141</v>
       </c>
@@ -17484,7 +17490,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R25" t="s">
         <v>146</v>
       </c>
@@ -17492,7 +17498,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R26" t="s">
         <v>148</v>
       </c>
@@ -17500,7 +17506,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R27" t="s">
         <v>150</v>
       </c>
@@ -17514,7 +17520,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q28" t="s">
         <v>122</v>
       </c>
@@ -17525,7 +17531,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R29" t="s">
         <v>142</v>
       </c>
@@ -17536,7 +17542,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q30" t="s">
         <v>123</v>
       </c>
@@ -17547,7 +17553,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R31" t="s">
         <v>143</v>
       </c>
@@ -17555,7 +17561,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q32" t="s">
         <v>128</v>
       </c>
@@ -17563,12 +17569,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="26:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z33" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="26:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z34" t="s">
         <v>150</v>
       </c>
@@ -17597,12 +17603,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="125e2131eddd38cce17ebc9527d7a9d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
@@ -17716,6 +17716,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
@@ -17725,21 +17731,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDF5CC58-C8DC-4B0B-B85F-BEEEE1EBC9AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17753,4 +17744,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>